<commit_message>
Improved center cavity check function
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49ECD370-CD96-402B-AC1D-F0C4E30E72D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDF61F0-1F3B-40E2-9BE9-F0041B4FD6B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,8 +19,46 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{75801F2C-D358-4A06-AF29-DB146EBFD8D6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+False negatives:
+- ? (edge too close)
+- ADB1_57 (crap near edge)
+- ADB1_76 (broken piece)
+- ADB1_80 (canny error, or edge sligthly broken)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Series</t>
   </si>
@@ -50,13 +88,19 @@
   </si>
   <si>
     <t>n false pos.</t>
+  </si>
+  <si>
+    <t>decreased symetry allowed relative error to 0.2</t>
+  </si>
+  <si>
+    <t>revert to 0.52</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +115,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -378,17 +435,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
@@ -484,6 +541,34 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>32</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>67</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="H1:I1"/>
@@ -495,5 +580,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
After concluding that previous line features were better. Will add multiple cavities exclusion feature.
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDF61F0-1F3B-40E2-9BE9-F0041B4FD6B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B65E38-B242-489C-8521-1B4EA0349005}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cavity detection algo" sheetId="1" r:id="rId1"/>
@@ -53,12 +53,37 @@
         </r>
       </text>
     </comment>
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{D951E769-D9E0-4317-BAF1-893A282B4535}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+False negatives:
+-ADB1_51</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Series</t>
   </si>
@@ -94,6 +119,9 @@
   </si>
   <si>
     <t>revert to 0.52</t>
+  </si>
+  <si>
+    <t>center diff is 0</t>
   </si>
 </sst>
 </file>
@@ -436,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,6 +597,20 @@
         <v>11</v>
       </c>
     </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>65</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="H1:I1"/>

</xml_diff>